<commit_message>
added total bill with gst to file
</commit_message>
<xml_diff>
--- a/reports/CustomerData.xlsx
+++ b/reports/CustomerData.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -405,6 +405,12 @@
       <c r="H1" t="str">
         <v>password</v>
       </c>
+      <c r="I1" t="str">
+        <v>checkOutDate</v>
+      </c>
+      <c r="J1" t="str">
+        <v>totalBill</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -426,15 +432,21 @@
         <v>2</v>
       </c>
       <c r="G2" t="str">
-        <v>2021-10-03T18:01:27.838Z</v>
+        <v>2021-10-04T18:18:33.152Z</v>
       </c>
       <c r="H2" t="str">
         <v>pratik123</v>
+      </c>
+      <c r="I2" t="str">
+        <v>2021-10-04T19:24:43.416Z</v>
+      </c>
+      <c r="J2">
+        <v>767</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>